<commit_message>
Overall Changes and Generation of new data
</commit_message>
<xml_diff>
--- a/data/biolog_results/plate_readout_categorizations.xlsx
+++ b/data/biolog_results/plate_readout_categorizations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentsrwthaachende-my.sharepoint.com/personal/ycy3t7jjvtr9b5h8_students_rwth-aachen_de/Documents/RWTH/Biotechnologie M. Sc/Masterarbeit/BIOLOG/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentsrwthaachende-my.sharepoint.com/personal/ycy3t7jjvtr9b5h8_students_rwth-aachen_de/Documents/RWTH/Biotechnologie M. Sc/Masterarbeit/lmurinus_gem/data/biolog_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1002" documentId="8_{064C2167-E200-447C-8061-CB3944B3AACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50FB3298-F36F-4EA7-B93E-EE34874E6550}"/>
+  <xr:revisionPtr revIDLastSave="1635" documentId="8_{064C2167-E200-447C-8061-CB3944B3AACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65365CA6-27EC-4AAA-B79B-D14674E1774F}"/>
   <bookViews>
-    <workbookView xWindow="15435" yWindow="540" windowWidth="19200" windowHeight="21000" xr2:uid="{20CE4D18-2B3B-4AED-9EDB-990B5DA742DE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{20CE4D18-2B3B-4AED-9EDB-990B5DA742DE}"/>
   </bookViews>
   <sheets>
     <sheet name="BIOLOG" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2351" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2939" uniqueCount="207">
   <si>
     <t>A01</t>
   </si>
@@ -655,6 +655,9 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>23-42</t>
   </si>
 </sst>
 </file>
@@ -704,7 +707,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -732,11 +735,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -745,6 +759,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,14 +820,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -848,7 +861,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -954,7 +967,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1096,7 +1109,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1104,10 +1117,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DEC020-CC51-413B-9599-E8757064AC86}">
-  <dimension ref="A1:CU22"/>
+  <dimension ref="A1:CU28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BQ1" workbookViewId="0">
-      <selection activeCell="BY29" sqref="BY29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7395,306 +7408,2100 @@
       </c>
     </row>
     <row r="22" spans="1:99" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="9">
         <v>24</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="P22" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="T22" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="U22" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="V22" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="W22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="X22" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="Y22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="Z22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AA22" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="AB22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AC22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AD22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AE22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AF22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AG22" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="AH22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AI22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AJ22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AK22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AL22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AM22" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="AN22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AO22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AP22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AQ22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AR22" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="AS22" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="AT22" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="AU22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AV22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AW22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AX22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AY22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AZ22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BA22" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="BB22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BC22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BD22" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="BE22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BF22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BG22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BH22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BI22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BJ22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BK22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BL22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BM22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BN22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BO22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BP22" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="BQ22" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="BR22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BS22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BT22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BU22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BV22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BW22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BX22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BY22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="BZ22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="CA22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="CB22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="CC22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="CD22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="CE22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="CF22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="CG22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="CH22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="CI22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="CJ22" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="CK22" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="CL22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="CM22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="CN22" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="CO22" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="CP22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="CQ22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="CR22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="CS22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="CT22" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="CU22" s="4" t="s">
+      <c r="D22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="M22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="N22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="O22" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="P22" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="R22" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="S22" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="T22" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="U22" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="V22" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="W22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="X22" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="Y22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="Z22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AA22" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="AB22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AC22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AD22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AE22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AF22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AG22" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="AH22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AI22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AJ22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AK22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AL22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AM22" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="AN22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AO22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AP22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AQ22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AR22" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="AS22" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT22" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="AU22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AV22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AW22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AX22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AY22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="AZ22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BA22" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="BB22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BC22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BD22" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="BE22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BF22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BG22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BH22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BI22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BJ22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BK22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BL22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BM22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BN22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BO22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BP22" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="BQ22" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="BR22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BS22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BT22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BU22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BV22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BW22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BX22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BY22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BZ22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="CA22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="CB22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="CC22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="CD22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="CE22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="CF22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="CG22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="CH22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="CI22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="CJ22" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="CK22" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="CL22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="CM22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="CN22" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="CO22" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="CP22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="CQ22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="CR22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="CS22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="CT22" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="CU22" s="9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="23" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B23" s="9">
+        <v>5</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="J23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="K23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="L23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="M23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="N23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="O23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="P23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="R23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="S23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="T23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="U23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="V23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="W23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="X23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="Y23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="Z23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AA23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AB23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AC23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AD23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AE23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AF23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AG23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AH23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AI23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AJ23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AK23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AL23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AM23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AN23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AO23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AP23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AQ23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AR23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AS23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AU23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AV23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AW23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AX23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AY23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AZ23" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BB23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BC23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BD23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BE23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BF23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BG23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BH23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BI23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BJ23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BK23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BL23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BM23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BN23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BO23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BP23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BQ23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BR23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BS23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BT23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BU23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BV23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BW23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BX23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BY23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BZ23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CA23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CB23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CC23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CD23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CE23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CF23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CG23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CH23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CI23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CJ23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CK23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CL23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CM23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CN23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CO23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CP23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CQ23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CR23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CS23" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CT23" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CU23" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B24" s="9">
+        <v>5</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="K24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="L24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="M24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="N24" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="O24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="P24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q24" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="R24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="S24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="T24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="U24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="V24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="W24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="X24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="Y24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="Z24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AA24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AB24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AC24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AD24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AE24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AF24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AG24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AH24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AI24" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AJ24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AK24" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AL24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AM24" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AN24" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AO24" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AP24" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AQ24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AR24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AS24" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AU24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AV24" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AW24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AX24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AY24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AZ24" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA24" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BB24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BC24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BD24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BE24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BF24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BG24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BH24" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BI24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BJ24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BK24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BL24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BM24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BN24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BO24" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BP24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BQ24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BR24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BS24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BT24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BU24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BV24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BW24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BX24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BY24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BZ24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CA24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CB24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CC24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CD24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CE24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CF24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CG24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CH24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CI24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CJ24" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CK24" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CL24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CM24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CN24" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CO24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CP24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CQ24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CR24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CS24" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CT24" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CU24" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B25" s="9">
+        <v>5</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="K25" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="L25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="M25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="N25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="O25" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="P25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="R25" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="S25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="T25" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="U25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="V25" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="W25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="X25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="Y25" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="Z25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AA25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AB25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AC25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AD25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AE25" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AF25" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AG25" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AH25" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AI25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AJ25" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AK25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AL25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AM25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AN25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AO25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AP25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AQ25" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AR25" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AS25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AU25" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AV25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AW25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AX25" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AY25" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AZ25" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BB25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BC25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BD25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BE25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BF25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BG25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BH25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BI25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BJ25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BK25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BL25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BM25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BN25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BO25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BP25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BQ25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BR25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BS25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BT25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BU25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BV25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BW25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BX25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BY25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BZ25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CA25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CB25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CC25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CD25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CE25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CF25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CG25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CH25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CI25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CJ25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CK25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CL25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CM25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CN25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CO25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CP25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CQ25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CR25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CS25" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CT25" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CU25" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B26" s="9">
+        <v>7</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="K26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="L26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="M26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="N26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="O26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="P26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="R26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="S26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="T26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="U26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="V26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="W26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="X26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="Y26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="Z26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AA26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AB26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AC26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AD26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AE26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AF26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AG26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AH26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AI26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AJ26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AK26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AL26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AM26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AN26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AO26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AP26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AQ26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AR26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AS26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AU26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AV26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AW26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AX26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AY26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AZ26" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BB26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BC26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BD26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BE26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BF26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BG26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BH26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BI26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BJ26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BK26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BL26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BM26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BN26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BO26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BP26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BQ26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BR26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BS26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BT26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BU26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BV26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BW26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BX26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BY26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BZ26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CA26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CB26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CC26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CD26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CE26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CF26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CG26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CH26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CI26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CJ26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CK26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CL26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CM26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CN26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CO26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CP26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CQ26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CR26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CS26" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CT26" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CU26" s="10" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="27" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B27" s="9">
+        <v>7</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="K27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="L27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="M27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="N27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="O27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="P27" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q27" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="R27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="S27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="T27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="U27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="V27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="W27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="X27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="Y27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="Z27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AA27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AB27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AC27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AD27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AE27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AF27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AG27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AH27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AI27" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AJ27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AK27" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AL27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AM27" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AN27" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AO27" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AP27" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AQ27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AR27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AS27" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AU27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AV27" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AW27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AX27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AY27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AZ27" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA27" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BB27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BC27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BD27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BE27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BF27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BG27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BH27" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BI27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BJ27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BK27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BL27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BM27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BN27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BO27" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BP27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BQ27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BR27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BS27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BT27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BU27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BV27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BW27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BX27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BY27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BZ27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CA27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CB27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CC27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CD27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CE27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CF27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CG27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CH27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CI27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CJ27" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CK27" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CL27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CM27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CN27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CO27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CP27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CQ27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CR27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CS27" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CT27" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CU27" s="10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="1:99" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="B28" s="9">
+        <v>7</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="K28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="L28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="M28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="N28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="O28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="P28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="R28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="S28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="T28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="U28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="V28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="W28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="X28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="Y28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="Z28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AA28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AB28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AC28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AD28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AE28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AF28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AG28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AH28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AI28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AJ28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AK28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AL28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AM28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AN28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AO28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AP28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AQ28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AR28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AS28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AT28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="AU28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AV28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AW28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="AX28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AY28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="AZ28" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="BA28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BB28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BC28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BD28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BE28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BF28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BG28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BH28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BI28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BJ28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BK28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BL28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BM28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BN28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BO28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="BP28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BQ28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BR28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BS28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BT28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BU28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BV28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BW28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BX28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BY28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="BZ28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CA28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CB28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CC28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CD28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CE28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CF28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CG28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CH28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CI28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CJ28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CK28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CL28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CM28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CN28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CO28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CP28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CQ28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CR28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CS28" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="CT28" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="CU28" s="10" t="s">
         <v>203</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:CU22">
+  <conditionalFormatting sqref="D2:CU28">
     <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="I">
       <formula>NOT(ISERROR(SEARCH("I",D2)))</formula>
     </cfRule>

</xml_diff>